<commit_message>
Update bacteria to North East Shelf
</commit_message>
<xml_diff>
--- a/Data/BacteriaConcentrations.xlsx
+++ b/Data/BacteriaConcentrations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/RawData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/AcidotropicDyes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7EFD6FC-6DE8-9A48-9AF1-DAB75311E6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C7EFD6FC-6DE8-9A48-9AF1-DAB75311E6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{080DA46F-4B1E-B247-9BCA-DD0FE3CB6FC1}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="3320" windowWidth="26040" windowHeight="14940" xr2:uid="{DA692A59-0EE0-4048-9DC2-01CAE299ECB5}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Cruise</t>
   </si>
   <si>
-    <t>New England Shelf</t>
-  </si>
-  <si>
     <t>Night</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>North East Shelf</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,7 +496,7 @@
         <v>1389463.7736146227</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -511,7 +511,7 @@
         <v>1658391.9324743629</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -522,13 +522,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2">
         <v>948537.84114906273</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -539,13 +539,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2">
         <v>1123099.4355017927</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -556,13 +556,13 @@
         <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2">
         <v>959005.65093918261</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -573,13 +573,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2">
         <v>759376.83334708272</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -590,13 +590,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="2">
         <v>932852.4181037728</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -607,13 +607,13 @@
         <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="2">
         <v>1497003.4218700328</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -624,13 +624,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="2">
         <v>1290757.9731804528</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -641,13 +641,13 @@
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="2">
         <v>1140499.4109197927</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -658,13 +658,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="2">
         <v>1019075.1238217327</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -675,13 +675,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="2">
         <v>1505273.7695569228</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -692,13 +692,13 @@
         <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="2">
         <v>1715724.6022898727</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -709,13 +709,13 @@
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="2">
         <v>1219750.1574847428</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -726,13 +726,13 @@
         <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" s="2">
         <v>1145055.9627075728</v>
       </c>
       <c r="E16" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -743,13 +743,13 @@
         <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" s="2">
         <v>1759052.5387501728</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -760,13 +760,13 @@
         <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" s="2">
         <v>1858909.0726698327</v>
       </c>
       <c r="E18" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -779,7 +779,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -792,12 +792,12 @@
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
       <c r="E20" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -807,12 +807,12 @@
         <v>984319.14641151298</v>
       </c>
       <c r="E21" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22">
         <v>19</v>
@@ -822,7 +822,7 @@
         <v>1933423.4119158529</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -833,13 +833,13 @@
         <v>8.5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="4">
         <v>371642.77600000001</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -850,13 +850,13 @@
         <v>8.5</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" s="4">
         <v>490596.967</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -867,13 +867,13 @@
         <v>8.5</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25" s="4">
         <v>426256.78200000001</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -884,13 +884,13 @@
         <v>16.600000000000001</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" s="4">
         <v>854058.53599999996</v>
       </c>
       <c r="E26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -901,13 +901,13 @@
         <v>16.600000000000001</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D27" s="4">
         <v>835412.527</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -918,13 +918,13 @@
         <v>16.600000000000001</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28" s="4">
         <v>769663.13100000005</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -935,13 +935,13 @@
         <v>50.4</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D29" s="4">
         <v>974444.76699999999</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -952,13 +952,13 @@
         <v>50.4</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D30" s="4">
         <v>875427.30299999996</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -969,13 +969,13 @@
         <v>50.4</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D31" s="4">
         <v>893196.39300000004</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -986,13 +986,13 @@
         <v>7.7</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32" s="4">
         <v>338137.217</v>
       </c>
       <c r="E32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1003,13 +1003,13 @@
         <v>7.7</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D33" s="4">
         <v>357910.80599999998</v>
       </c>
       <c r="E33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1020,13 +1020,13 @@
         <v>45.6</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D34" s="4">
         <v>914475.39500000002</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1037,13 +1037,13 @@
         <v>45.6</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D35" s="4">
         <v>922357.49600000004</v>
       </c>
       <c r="E35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1054,13 +1054,13 @@
         <v>7.7</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D36" s="4">
         <v>1060462.81</v>
       </c>
       <c r="E36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1071,13 +1071,13 @@
         <v>7.7</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D37" s="4">
         <v>990391.18299999996</v>
       </c>
       <c r="E37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1088,13 +1088,13 @@
         <v>7.7</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D38" s="4">
         <v>1019293.9</v>
       </c>
       <c r="E38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1105,13 +1105,13 @@
         <v>15</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D39" s="4">
         <v>891069.06599999999</v>
       </c>
       <c r="E39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1122,13 +1122,13 @@
         <v>15</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D40" s="4">
         <v>930021.42700000003</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1139,13 +1139,13 @@
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D41" s="4">
         <v>876478.34</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1156,13 +1156,13 @@
         <v>22.8</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D42" s="4">
         <v>673696.34699999995</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1173,13 +1173,13 @@
         <v>22.8</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D43" s="4">
         <v>700196.17099999997</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1190,13 +1190,13 @@
         <v>22.8</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D44" s="4">
         <v>720749.92700000003</v>
       </c>
       <c r="E44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1207,13 +1207,13 @@
         <v>8</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D45" s="4">
         <v>443989.772</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1224,13 +1224,13 @@
         <v>8</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D46" s="4">
         <v>513176.005</v>
       </c>
       <c r="E46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1241,13 +1241,13 @@
         <v>8</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D47" s="4">
         <v>464565.50300000003</v>
       </c>
       <c r="E47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1258,13 +1258,13 @@
         <v>15.7</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D48" s="4">
         <v>496905.42099999997</v>
       </c>
       <c r="E48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1275,13 +1275,13 @@
         <v>15.7</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D49" s="4">
         <v>433105.712</v>
       </c>
       <c r="E49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1292,13 +1292,13 @@
         <v>15.7</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D50" s="4">
         <v>429590.13799999998</v>
       </c>
       <c r="E50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1309,13 +1309,13 @@
         <v>47.3</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D51" s="4">
         <v>441435.64399999997</v>
       </c>
       <c r="E51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1326,13 +1326,13 @@
         <v>47.3</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D52" s="4">
         <v>555306.86</v>
       </c>
       <c r="E52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1343,13 +1343,13 @@
         <v>7.4</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D53" s="4">
         <v>381026.94199999998</v>
       </c>
       <c r="E53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1360,13 +1360,13 @@
         <v>7.4</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D54" s="4">
         <v>317831.799</v>
       </c>
       <c r="E54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1377,13 +1377,13 @@
         <v>14.4</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D55" s="4">
         <v>149001.20499999999</v>
       </c>
       <c r="E55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1394,13 +1394,13 @@
         <v>14.4</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D56" s="4">
         <v>116614.037</v>
       </c>
       <c r="E56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -1411,13 +1411,13 @@
         <v>22.1</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D57" s="4">
         <v>351865.21799999999</v>
       </c>
       <c r="E57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -1428,13 +1428,13 @@
         <v>22.1</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D58" s="4">
         <v>347441.39500000002</v>
       </c>
       <c r="E58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -1445,13 +1445,13 @@
         <v>22.1</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D59" s="4">
         <v>367907.39500000002</v>
       </c>
       <c r="E59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -1462,13 +1462,13 @@
         <v>7.4</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D60" s="4">
         <v>1036428.52</v>
       </c>
       <c r="E60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -1479,13 +1479,13 @@
         <v>7.4</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D61" s="4">
         <v>959287.26199999999</v>
       </c>
       <c r="E61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -1496,13 +1496,13 @@
         <v>7.4</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D62" s="4">
         <v>909329.74899999995</v>
       </c>
       <c r="E62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -1513,13 +1513,13 @@
         <v>14.4</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D63" s="4">
         <v>911170.33400000003</v>
       </c>
       <c r="E63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -1530,13 +1530,13 @@
         <v>14.4</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D64" s="4">
         <v>866849.72600000002</v>
       </c>
       <c r="E64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -1547,13 +1547,13 @@
         <v>14.4</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D65" s="4">
         <v>869467.28500000003</v>
       </c>
       <c r="E65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -1564,13 +1564,13 @@
         <v>21.9</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D66" s="4">
         <v>736035.66700000002</v>
       </c>
       <c r="E66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -1581,13 +1581,13 @@
         <v>21.9</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D67" s="4">
         <v>674515.51300000004</v>
       </c>
       <c r="E67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -1598,13 +1598,13 @@
         <v>21.9</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D68" s="4">
         <v>730806.179</v>
       </c>
       <c r="E68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -1615,13 +1615,13 @@
         <v>7.4</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D69" s="4">
         <v>912927.25399999996</v>
       </c>
       <c r="E69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -1632,13 +1632,13 @@
         <v>7.4</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D70" s="4">
         <v>813150.12300000002</v>
       </c>
       <c r="E70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -1649,13 +1649,13 @@
         <v>7.4</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D71" s="4">
         <v>907793.24800000002</v>
       </c>
       <c r="E71" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -1666,13 +1666,13 @@
         <v>14.4</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D72" s="4">
         <v>704264.90800000005</v>
       </c>
       <c r="E72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -1683,13 +1683,13 @@
         <v>14.4</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D73" s="4">
         <v>723969.18599999999</v>
       </c>
       <c r="E73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -1700,13 +1700,13 @@
         <v>14.4</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D74" s="4">
         <v>689907.39599999995</v>
       </c>
       <c r="E74" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -1717,13 +1717,13 @@
         <v>21.9</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D75" s="4">
         <v>738304.75399999996</v>
       </c>
       <c r="E75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -1734,13 +1734,13 @@
         <v>21.9</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D76" s="4">
         <v>677017.29200000002</v>
       </c>
       <c r="E76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -1751,13 +1751,13 @@
         <v>21.9</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D77" s="4">
         <v>604095.75800000003</v>
       </c>
       <c r="E77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -1768,13 +1768,13 @@
         <v>11.8</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D78" s="4">
         <v>522691.05900000001</v>
       </c>
       <c r="E78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -1785,13 +1785,13 @@
         <v>11.8</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D79" s="4">
         <v>515083.51400000002</v>
       </c>
       <c r="E79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -1802,13 +1802,13 @@
         <v>11.8</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D80" s="4">
         <v>489147.45500000002</v>
       </c>
       <c r="E80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -1819,13 +1819,13 @@
         <v>22.4</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D81" s="4">
         <v>427808.73100000003</v>
       </c>
       <c r="E81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -1836,13 +1836,13 @@
         <v>22.4</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D82" s="4">
         <v>501200.397</v>
       </c>
       <c r="E82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -1853,13 +1853,13 @@
         <v>33.9</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D83" s="4">
         <v>503749.31</v>
       </c>
       <c r="E83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -1870,13 +1870,13 @@
         <v>33.9</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D84" s="4">
         <v>414996.06199999998</v>
       </c>
       <c r="E84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -1887,13 +1887,13 @@
         <v>33.9</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D85" s="4">
         <v>410653.02</v>
       </c>
       <c r="E85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -1904,13 +1904,13 @@
         <v>7.4</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D86" s="4">
         <v>940495.71699999995</v>
       </c>
       <c r="E86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -1921,13 +1921,13 @@
         <v>7.4</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D87" s="4">
         <v>907026.16799999995</v>
       </c>
       <c r="E87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -1938,13 +1938,13 @@
         <v>7.4</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D88" s="4">
         <v>997946.31499999994</v>
       </c>
       <c r="E88" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -1955,13 +1955,13 @@
         <v>14.5</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D89" s="4">
         <v>471504.44400000002</v>
       </c>
       <c r="E89" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -1972,13 +1972,13 @@
         <v>14.5</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D90" s="4">
         <v>428757.66</v>
       </c>
       <c r="E90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -1989,13 +1989,13 @@
         <v>14.5</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D91" s="4">
         <v>467074.67700000003</v>
       </c>
       <c r="E91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2006,13 +2006,13 @@
         <v>7.4</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D92" s="4">
         <v>1542260.84</v>
       </c>
       <c r="E92" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2023,13 +2023,13 @@
         <v>7.4</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D93" s="4">
         <v>1454528.5</v>
       </c>
       <c r="E93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -2040,13 +2040,13 @@
         <v>7.4</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D94" s="4">
         <v>1412960.89</v>
       </c>
       <c r="E94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -2057,13 +2057,13 @@
         <v>14.4</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D95" s="4">
         <v>829693.31200000003</v>
       </c>
       <c r="E95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -2074,13 +2074,13 @@
         <v>14.4</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D96" s="4">
         <v>966711.96600000001</v>
       </c>
       <c r="E96" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -2091,13 +2091,13 @@
         <v>14.4</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D97" s="4">
         <v>1035292.32</v>
       </c>
       <c r="E97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>